<commit_message>
added headless chrome execution option
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/Shakedown 1.xlsx
+++ b/src/test/java/dataEngine/Shakedown 1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -297,9 +297,6 @@
     <t>TS_029</t>
   </si>
   <si>
-    <t>waitFor5</t>
-  </si>
-  <si>
     <t>TS_030</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>btn_Close</t>
   </si>
   <si>
-    <t>TS_032</t>
-  </si>
-  <si>
     <t>COMP</t>
   </si>
   <si>
@@ -379,6 +373,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -483,8 +480,36 @@
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
+    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -780,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,10 +874,10 @@
         <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="I2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -876,10 +901,10 @@
         <v>19</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -906,7 +931,7 @@
         <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -932,7 +957,7 @@
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -955,7 +980,7 @@
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -978,7 +1003,7 @@
         <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1001,7 +1026,7 @@
         <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1024,7 +1049,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1047,7 +1072,7 @@
         <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1070,7 +1095,7 @@
         <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1116,7 +1141,7 @@
         <v>54</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1139,7 +1164,7 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1162,7 +1187,7 @@
         <v>60</v>
       </c>
       <c r="I15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,7 +1210,7 @@
         <v>13</v>
       </c>
       <c r="I16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1208,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1231,7 +1256,7 @@
         <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1254,7 +1279,7 @@
         <v>68</v>
       </c>
       <c r="I19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,7 +1302,7 @@
         <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1294,13 +1319,13 @@
         <v>74</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H21" s="6">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1324,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1347,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1369,7 +1394,7 @@
         <v>15</v>
       </c>
       <c r="I24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1389,10 +1414,10 @@
         <v>19</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1415,7 +1440,7 @@
         <v>81</v>
       </c>
       <c r="I26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1438,7 +1463,7 @@
         <v>72</v>
       </c>
       <c r="I27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1452,7 +1477,7 @@
         <v>80</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>29</v>
@@ -1461,7 +1486,7 @@
         <v>13</v>
       </c>
       <c r="I28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1484,7 +1509,7 @@
         <v>13</v>
       </c>
       <c r="I29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1492,7 +1517,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>80</v>
@@ -1507,7 +1532,7 @@
         <v>13</v>
       </c>
       <c r="I30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1515,10 +1540,10 @@
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>80</v>
@@ -1533,7 +1558,7 @@
         <v>13</v>
       </c>
       <c r="I31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1546,66 +1571,66 @@
       <c r="D32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H32" s="6">
-        <v>1</v>
+      <c r="F32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="I32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>117</v>
+        <v>29</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I33" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="I34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1616,19 +1641,19 @@
         <v>80</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="I35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1664,7 @@
         <v>80</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>29</v>
@@ -1648,10 +1673,10 @@
         <v>13</v>
       </c>
       <c r="I36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1662,7 +1687,7 @@
         <v>80</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>29</v>
@@ -1671,122 +1696,99 @@
         <v>13</v>
       </c>
       <c r="I37" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="I38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="I39" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I40" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test data to add headless chrome option
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/Shakedown 1.xlsx
+++ b/src/test/java/dataEngine/Shakedown 1.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="10290" windowWidth="18195" xWindow="240" yWindow="30"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="18195" windowHeight="10290"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="120">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>openBrowser</t>
-  </si>
-  <si>
-    <t>Mozilla</t>
   </si>
   <si>
     <t>TS_002</t>
@@ -385,7 +382,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,31 +450,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -504,10 +500,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -523,10 +519,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -684,7 +680,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -693,13 +689,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -709,7 +705,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -718,7 +714,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -727,7 +723,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -737,12 +733,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -773,7 +769,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -792,7 +788,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -804,24 +800,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="39.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="24.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -874,10 +870,10 @@
         <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -885,26 +881,26 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -912,26 +908,26 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="I4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -939,25 +935,25 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -965,22 +961,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -988,22 +984,22 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1011,22 +1007,22 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1034,22 +1030,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,22 +1053,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="I10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1080,22 +1076,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1103,22 +1099,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1126,22 +1122,22 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="I13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1149,22 +1145,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,22 +1168,22 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1195,22 +1191,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1218,22 +1214,22 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1241,22 +1237,22 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1264,22 +1260,22 @@
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="I19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1287,22 +1283,22 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="I20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1310,22 +1306,22 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21" s="6">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1333,23 +1329,23 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="6">
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1357,7 +1353,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -1366,13 +1362,13 @@
         <v>13</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H23" s="6">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1380,10 +1376,10 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="6"/>
@@ -1391,10 +1387,10 @@
         <v>14</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="I24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1402,22 +1398,22 @@
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1425,22 +1421,22 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="I26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1448,22 +1444,22 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="H27" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1471,22 +1467,22 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1494,22 +1490,22 @@
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1517,22 +1513,22 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1540,25 +1536,25 @@
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1566,22 +1562,22 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F32" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="H32" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1589,22 +1585,22 @@
         <v>9</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1612,22 +1608,22 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H34" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1635,22 +1631,22 @@
         <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1658,22 +1654,22 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1681,22 +1677,22 @@
         <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1704,22 +1700,22 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H38" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1727,22 +1723,22 @@
         <v>9</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1750,22 +1746,22 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1773,50 +1769,50 @@
         <v>9</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="H41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>